<commit_message>
Adding command line arguments option. it is working fine on oneplus device, srivani and myself verified it.
</commit_message>
<xml_diff>
--- a/Xindus_PerfReport_Androbench.xlsx
+++ b/Xindus_PerfReport_Androbench.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>seq_read</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>iteration 1</t>
-  </si>
-  <si>
-    <t>iteration 2</t>
   </si>
 </sst>
 </file>
@@ -146,35 +143,29 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>Sheet1!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1461</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1451</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1442</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1437</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -201,35 +192,29 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:f>Sheet1!$C$2:$C$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>393</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>392</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>398</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,35 +241,29 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:f>Sheet1!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>183</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -311,35 +290,29 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$4</c:f>
+              <c:f>Sheet1!$E$2:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -366,35 +339,29 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$4</c:f>
+              <c:f>Sheet1!$F$2:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2746</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2739</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
                   <c:v>2722</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2654</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -421,35 +388,29 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$4</c:f>
+              <c:f>Sheet1!$G$2:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>4430</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4292</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4355</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4351</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4287</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -476,35 +437,29 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$4</c:f>
+              <c:f>Sheet1!$H$2:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>5135</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5240</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4953</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,7 +865,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -944,25 +899,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1461</v>
+        <v>1437</v>
       </c>
       <c r="C2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D2">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E2">
         <v>27</v>
       </c>
       <c r="F2">
-        <v>2746</v>
+        <v>2722</v>
       </c>
       <c r="G2">
-        <v>4430</v>
+        <v>4351</v>
       </c>
       <c r="H2">
-        <v>5135</v>
+        <v>5001</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -970,51 +925,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1451</v>
+        <v>1444</v>
       </c>
       <c r="C3">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="D3">
         <v>173</v>
       </c>
       <c r="E3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F3">
-        <v>2739</v>
+        <v>2654</v>
       </c>
       <c r="G3">
-        <v>4292</v>
+        <v>4287</v>
       </c>
       <c r="H3">
-        <v>5240</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>1442</v>
-      </c>
-      <c r="C4">
-        <v>398</v>
-      </c>
-      <c r="D4">
-        <v>179</v>
-      </c>
-      <c r="E4">
-        <v>27</v>
-      </c>
-      <c r="F4">
-        <v>2722</v>
-      </c>
-      <c r="G4">
-        <v>4355</v>
-      </c>
-      <c r="H4">
-        <v>4953</v>
+        <v>4928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding screenshots as user input arg.
</commit_message>
<xml_diff>
--- a/Xindus_PerfReport_Androbench.xlsx
+++ b/Xindus_PerfReport_Androbench.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>seq_read</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>iteration 1</t>
+  </si>
+  <si>
+    <t>iteration 2</t>
   </si>
 </sst>
 </file>
@@ -143,29 +146,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$3</c:f>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1437</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1444</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -192,29 +201,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$3</c:f>
+              <c:f>Sheet1!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -241,29 +256,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$3</c:f>
+              <c:f>Sheet1!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -290,29 +311,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$3</c:f>
+              <c:f>Sheet1!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -339,29 +366,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$3</c:f>
+              <c:f>Sheet1!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>2722</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2654</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -388,29 +421,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$3</c:f>
+              <c:f>Sheet1!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4351</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4287</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,29 +476,35 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>iteration 0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>iteration 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iteration 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$3</c:f>
+              <c:f>Sheet1!$H$2:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>5001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -865,7 +910,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -946,6 +991,32 @@
         <v>4928</v>
       </c>
     </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1443</v>
+      </c>
+      <c r="C4">
+        <v>399</v>
+      </c>
+      <c r="D4">
+        <v>181</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>2716</v>
+      </c>
+      <c r="G4">
+        <v>4330</v>
+      </c>
+      <c r="H4">
+        <v>5139</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>